<commit_message>
aqui ele já cria e verifica da base
</commit_message>
<xml_diff>
--- a/conta.xlsx
+++ b/conta.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brunna\Desktop\Nova pasta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INTECELERI\Documents\code\automa-o_contas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DB1804-8C03-431A-8324-72602EFAADA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966973CC-8577-44FC-B69E-F08180B60676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="2115" windowWidth="20730" windowHeight="11760" xr2:uid="{ABB5D061-89DC-45B2-A3EE-1C28E651AA0E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ABB5D061-89DC-45B2-A3EE-1C28E651AA0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,76 +25,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
-  <si>
-    <t>raelma@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>beatriz.ferreira@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>danubia.rodrigues@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>anderson.ferreira@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>arlene.cruz@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>ana.moreira@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>erica.santos@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>alessandra.damasceno@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>cleiton.goncalves@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>signe.farias@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>neuziane.veiga@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>neilza.tavares@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>neire.faial@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>anselmo.damasceno@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>larissa.pinheiro@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>elane.souza@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>edirlane.pinheiro@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>raimundo.oliveira@docente.semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
-  <si>
-    <t>elaine.amaral@semed.limoeirodoajuru.pa.gov.br</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>aline.ribeiro@docente.semec.belem.pa.gov.br</t>
+  </si>
+  <si>
+    <t>andreza.silva@semec.belem.pa.gov.br</t>
+  </si>
+  <si>
+    <t>claudia.moreira@docente.semec.belem.pa.gov.br</t>
+  </si>
+  <si>
+    <t>cleonice.silva@semec.belem.pa.gov.br</t>
+  </si>
+  <si>
+    <t>edelra.nunes@semec.belem.pa.gov.br</t>
+  </si>
+  <si>
+    <t>juliana.tourinho@semec.belem.pa.gov.br</t>
+  </si>
+  <si>
+    <t>karina.portal@semec.belem.pa.gov.br</t>
+  </si>
+  <si>
+    <t>nilcilene.dias@docente.semec.belem.pa.gov.br</t>
+  </si>
+  <si>
+    <t>raimunda.barriga@semec.belem.pa.gov.br</t>
+  </si>
+  <si>
+    <t>rakel.goes@docente.semec.belem.pa.gov.br</t>
+  </si>
+  <si>
+    <t>renata.mota@docente.semec.belem.pa.gov.br</t>
+  </si>
+  <si>
+    <t>roseane.tunas@semec.belem.pa.gov.br</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,13 +111,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -436,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2D7932-8C5F-443D-AEDC-3E03D149EE1D}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,108 +447,71 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>